<commit_message>
finished first complete verson V1.0
</commit_message>
<xml_diff>
--- a/Naderer/tests/Tests-WS.xlsx
+++ b/Naderer/tests/Tests-WS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private\Git\bacc\Naderer\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92578C3E-9F1E-4B7A-9EAB-978268EE4FBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A73A54-9E6B-43C8-B1DD-E96C625479FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9375" activeTab="2" xr2:uid="{EE9D9061-8DB4-44C4-ADBA-C12DA1E57691}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
   <si>
     <t>AL</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Testlauf 2</t>
+  </si>
+  <si>
+    <t>C/AL</t>
   </si>
 </sst>
 </file>
@@ -1131,7 +1134,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="de-AT" baseline="0"/>
-              <a:t> für 10 Kunden me je 10.000 Posten - Erstermittlung</a:t>
+              <a:t> für 10 Kunden mit je 10.000 Posten - Erstermittlung</a:t>
             </a:r>
             <a:endParaRPr lang="de-AT"/>
           </a:p>
@@ -1182,7 +1185,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C/AL .NET</c:v>
+                  <c:v>C/AL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1622,7 +1625,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1666,7 +1669,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="de-AT" baseline="0"/>
-              <a:t> für 10 Kunden me je 10.000 Posten - Zwischenspeicher</a:t>
+              <a:t> für 10 Kunden mit je 10.000 Posten - Zwischenspeicher</a:t>
             </a:r>
             <a:endParaRPr lang="de-AT"/>
           </a:p>
@@ -1717,7 +1720,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C/AL .NET</c:v>
+                  <c:v>C/AL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4433,13 +4436,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>52387</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>112971</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4466,16 +4469,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>77530</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4915,8 +4918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D8CF38-910F-4B3B-A59A-C18F8E0A17EB}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4967,7 +4970,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>2.5999999999999999E-2</v>
@@ -4990,7 +4993,7 @@
         <v>1.2247448713915887E-3</v>
       </c>
       <c r="I2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J2">
         <v>1.7000000000000001E-2</v>
@@ -5063,6 +5066,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>